<commit_message>
Visualization of data when applying TDA by R
</commit_message>
<xml_diff>
--- a/input_data/maru-ten.xlsx
+++ b/input_data/maru-ten.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nakayamarina/Desktop/nakayama/portfolio/tda/input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/TDA_tryweb/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37100" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,16 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="1"/>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -78,11 +69,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -360,25 +348,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="31" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="A1">
+        <v>3</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -386,7 +374,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -394,15 +382,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -410,15 +398,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -426,7 +414,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -434,15 +422,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -450,10 +438,10 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
@@ -466,7 +454,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -474,17 +462,9 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15">
         <v>6</v>
       </c>
     </row>

</xml_diff>